<commit_message>
DCIT 21 Midterm Updates
</commit_message>
<xml_diff>
--- a/DCIT 21 - IT 1C/LEC AND LAB - IT 1C.xlsx
+++ b/DCIT 21 - IT 1C/LEC AND LAB - IT 1C.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="REGISTRATION" sheetId="1" r:id="rId1"/>
@@ -3887,8 +3887,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6110,9 +6110,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:CU70"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J22" sqref="J22"/>
+      <selection pane="topRight" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7064,14 +7064,16 @@
         <f>CONCATENATE(REGISTRATION!C11," ",REGISTRATION!D11," ",REGISTRATION!E11)</f>
         <v>Ambulo Anne Jelica R</v>
       </c>
-      <c r="D10" s="107"/>
+      <c r="D10" s="107">
+        <v>35</v>
+      </c>
       <c r="E10" s="92">
         <f>(D10/$D$9)*100</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F10" s="95">
         <f t="shared" ref="F10:F41" si="0">IFERROR((E10*$F$7), " ")</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G10" s="107"/>
       <c r="H10" s="92" t="e">
@@ -7176,11 +7178,11 @@
       </c>
       <c r="BC10" s="98">
         <f>IFERROR(SUM(BB10,AU10,AN10,I10,F10),"")</f>
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="BD10" s="98">
         <f>IFERROR(ROUND(BC10,2),"")</f>
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="BE10" s="107"/>
       <c r="BF10" s="92" t="str">
@@ -7290,7 +7292,7 @@
       </c>
       <c r="CS10" s="104">
         <f>IFERROR(((CR10*0.6)+(BD10*0.4)),"")</f>
-        <v>5.2</v>
+        <v>11.200000000000001</v>
       </c>
       <c r="CT10" s="104">
         <f>IFERROR(VLOOKUP(CS10,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -7314,14 +7316,16 @@
         <f>CONCATENATE(REGISTRATION!C12," ",REGISTRATION!D12," ",REGISTRATION!E12)</f>
         <v>Amon Bryan Eriz C</v>
       </c>
-      <c r="D11" s="108"/>
+      <c r="D11" s="108">
+        <v>33</v>
+      </c>
       <c r="E11" s="92">
         <f>(D11/$D$9)*100</f>
-        <v>0</v>
+        <v>47.142857142857139</v>
       </c>
       <c r="F11" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14.142857142857141</v>
       </c>
       <c r="G11" s="108"/>
       <c r="H11" s="92" t="e">
@@ -7426,11 +7430,11 @@
       </c>
       <c r="BC11" s="98">
         <f t="shared" ref="BC11:BC70" si="18">IFERROR(SUM(BB11,AU11,AN11,I11,F11),"")</f>
-        <v>13</v>
+        <v>27.142857142857139</v>
       </c>
       <c r="BD11" s="98">
         <f t="shared" ref="BD11:BD70" si="19">IFERROR(ROUND(BC11,2),"")</f>
-        <v>13</v>
+        <v>27.14</v>
       </c>
       <c r="BE11" s="108"/>
       <c r="BF11" s="92" t="str">
@@ -7540,7 +7544,7 @@
       </c>
       <c r="CS11" s="104">
         <f t="shared" ref="CS11:CS22" si="41">IFERROR(((CR11*0.6)+(BD11*0.4)),"")</f>
-        <v>5.2</v>
+        <v>10.856000000000002</v>
       </c>
       <c r="CT11" s="104">
         <f>IFERROR(VLOOKUP(CS11,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -7564,14 +7568,16 @@
         <f>CONCATENATE(REGISTRATION!C13," ",REGISTRATION!D13," ",REGISTRATION!E13)</f>
         <v>Amutan Annalyn R</v>
       </c>
-      <c r="D12" s="108"/>
+      <c r="D12" s="108">
+        <v>58</v>
+      </c>
       <c r="E12" s="92">
         <f t="shared" ref="E12:E70" si="43">(D12/$D$9)*100</f>
-        <v>0</v>
+        <v>82.857142857142861</v>
       </c>
       <c r="F12" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>24.857142857142858</v>
       </c>
       <c r="G12" s="108"/>
       <c r="H12" s="92" t="e">
@@ -7676,11 +7682,11 @@
       </c>
       <c r="BC12" s="98">
         <f t="shared" si="18"/>
-        <v>15</v>
+        <v>39.857142857142861</v>
       </c>
       <c r="BD12" s="98">
         <f t="shared" si="19"/>
-        <v>15</v>
+        <v>39.86</v>
       </c>
       <c r="BE12" s="108"/>
       <c r="BF12" s="92" t="str">
@@ -7790,7 +7796,7 @@
       </c>
       <c r="CS12" s="104">
         <f t="shared" si="41"/>
-        <v>6</v>
+        <v>15.944000000000001</v>
       </c>
       <c r="CT12" s="104">
         <f>IFERROR(VLOOKUP(CS12,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -7814,14 +7820,16 @@
         <f>CONCATENATE(REGISTRATION!C14," ",REGISTRATION!D14," ",REGISTRATION!E14)</f>
         <v>Arevalo Jethro V</v>
       </c>
-      <c r="D13" s="108"/>
+      <c r="D13" s="108">
+        <v>44</v>
+      </c>
       <c r="E13" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>62.857142857142854</v>
       </c>
       <c r="F13" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18.857142857142854</v>
       </c>
       <c r="G13" s="108"/>
       <c r="H13" s="92" t="e">
@@ -7926,11 +7934,11 @@
       </c>
       <c r="BC13" s="98">
         <f t="shared" si="18"/>
-        <v>10</v>
+        <v>28.857142857142854</v>
       </c>
       <c r="BD13" s="98">
         <f t="shared" si="19"/>
-        <v>10</v>
+        <v>28.86</v>
       </c>
       <c r="BE13" s="108"/>
       <c r="BF13" s="92" t="str">
@@ -8040,7 +8048,7 @@
       </c>
       <c r="CS13" s="104">
         <f t="shared" si="41"/>
-        <v>4</v>
+        <v>11.544</v>
       </c>
       <c r="CT13" s="104">
         <f>IFERROR(VLOOKUP(CS13,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -8064,14 +8072,16 @@
         <f>CONCATENATE(REGISTRATION!C15," ",REGISTRATION!D15," ",REGISTRATION!E15)</f>
         <v>Baptista Jeffrey DC</v>
       </c>
-      <c r="D14" s="108"/>
+      <c r="D14" s="108">
+        <v>32</v>
+      </c>
       <c r="E14" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>45.714285714285715</v>
       </c>
       <c r="F14" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13.714285714285714</v>
       </c>
       <c r="G14" s="108"/>
       <c r="H14" s="92" t="e">
@@ -8176,11 +8186,11 @@
       </c>
       <c r="BC14" s="98">
         <f t="shared" si="18"/>
-        <v>14</v>
+        <v>27.714285714285715</v>
       </c>
       <c r="BD14" s="98">
         <f t="shared" si="19"/>
-        <v>14</v>
+        <v>27.71</v>
       </c>
       <c r="BE14" s="108"/>
       <c r="BF14" s="92" t="str">
@@ -8290,7 +8300,7 @@
       </c>
       <c r="CS14" s="104">
         <f t="shared" si="41"/>
-        <v>5.6000000000000005</v>
+        <v>11.084000000000001</v>
       </c>
       <c r="CT14" s="104">
         <f>IFERROR(VLOOKUP(CS14,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -8314,14 +8324,16 @@
         <f>CONCATENATE(REGISTRATION!C16," ",REGISTRATION!D16," ",REGISTRATION!E16)</f>
         <v>Baterna Kenneth M</v>
       </c>
-      <c r="D15" s="108"/>
+      <c r="D15" s="108">
+        <v>44</v>
+      </c>
       <c r="E15" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>62.857142857142854</v>
       </c>
       <c r="F15" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18.857142857142854</v>
       </c>
       <c r="G15" s="108"/>
       <c r="H15" s="92" t="e">
@@ -8426,11 +8438,11 @@
       </c>
       <c r="BC15" s="98">
         <f t="shared" si="18"/>
-        <v>15</v>
+        <v>33.857142857142854</v>
       </c>
       <c r="BD15" s="98">
         <f t="shared" si="19"/>
-        <v>15</v>
+        <v>33.86</v>
       </c>
       <c r="BE15" s="108"/>
       <c r="BF15" s="92" t="str">
@@ -8540,7 +8552,7 @@
       </c>
       <c r="CS15" s="104">
         <f t="shared" si="41"/>
-        <v>6</v>
+        <v>13.544</v>
       </c>
       <c r="CT15" s="104">
         <f>IFERROR(VLOOKUP(CS15,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -8564,14 +8576,16 @@
         <f>CONCATENATE(REGISTRATION!C17," ",REGISTRATION!D17," ",REGISTRATION!E17)</f>
         <v>Borja Ken G</v>
       </c>
-      <c r="D16" s="108"/>
+      <c r="D16" s="108">
+        <v>63</v>
+      </c>
       <c r="E16" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F16" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G16" s="108"/>
       <c r="H16" s="92" t="e">
@@ -8676,11 +8690,11 @@
       </c>
       <c r="BC16" s="98">
         <f t="shared" si="18"/>
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="BD16" s="98">
         <f t="shared" si="19"/>
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="BE16" s="108"/>
       <c r="BF16" s="92" t="str">
@@ -8790,7 +8804,7 @@
       </c>
       <c r="CS16" s="104">
         <f t="shared" si="41"/>
-        <v>6.8000000000000007</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="CT16" s="104">
         <f>IFERROR(VLOOKUP(CS16,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -9064,14 +9078,16 @@
         <f>CONCATENATE(REGISTRATION!C19," ",REGISTRATION!D19," ",REGISTRATION!E19)</f>
         <v>Buklatin Joseph Andrews A</v>
       </c>
-      <c r="D18" s="108"/>
+      <c r="D18" s="108">
+        <v>32</v>
+      </c>
       <c r="E18" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>45.714285714285715</v>
       </c>
       <c r="F18" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13.714285714285714</v>
       </c>
       <c r="G18" s="108"/>
       <c r="H18" s="92" t="e">
@@ -9176,11 +9192,11 @@
       </c>
       <c r="BC18" s="98">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>13.714285714285714</v>
       </c>
       <c r="BD18" s="98">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>13.71</v>
       </c>
       <c r="BE18" s="108"/>
       <c r="BF18" s="92" t="str">
@@ -9290,7 +9306,7 @@
       </c>
       <c r="CS18" s="104">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>5.4840000000000009</v>
       </c>
       <c r="CT18" s="104">
         <f>IFERROR(VLOOKUP(CS18,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -9314,14 +9330,16 @@
         <f>CONCATENATE(REGISTRATION!C20," ",REGISTRATION!D20," ",REGISTRATION!E20)</f>
         <v>Camitoc Anna Katrina A</v>
       </c>
-      <c r="D19" s="108"/>
+      <c r="D19" s="108">
+        <v>40</v>
+      </c>
       <c r="E19" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>57.142857142857139</v>
       </c>
       <c r="F19" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17.142857142857142</v>
       </c>
       <c r="G19" s="108"/>
       <c r="H19" s="92" t="e">
@@ -9426,11 +9444,11 @@
       </c>
       <c r="BC19" s="98">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>17.142857142857142</v>
       </c>
       <c r="BD19" s="98">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>17.14</v>
       </c>
       <c r="BE19" s="108"/>
       <c r="BF19" s="92" t="str">
@@ -9540,7 +9558,7 @@
       </c>
       <c r="CS19" s="104">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>6.8560000000000008</v>
       </c>
       <c r="CT19" s="104">
         <f>IFERROR(VLOOKUP(CS19,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -9564,14 +9582,16 @@
         <f>CONCATENATE(REGISTRATION!C21," ",REGISTRATION!D21," ",REGISTRATION!E21)</f>
         <v>Costelo Tyrone Jay A</v>
       </c>
-      <c r="D20" s="108"/>
+      <c r="D20" s="108">
+        <v>38</v>
+      </c>
       <c r="E20" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>54.285714285714285</v>
       </c>
       <c r="F20" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="G20" s="108"/>
       <c r="H20" s="92" t="e">
@@ -9676,11 +9696,11 @@
       </c>
       <c r="BC20" s="98">
         <f t="shared" si="18"/>
-        <v>10</v>
+        <v>26.285714285714285</v>
       </c>
       <c r="BD20" s="98">
         <f t="shared" si="19"/>
-        <v>10</v>
+        <v>26.29</v>
       </c>
       <c r="BE20" s="108"/>
       <c r="BF20" s="92" t="str">
@@ -9790,7 +9810,7 @@
       </c>
       <c r="CS20" s="104">
         <f t="shared" si="41"/>
-        <v>4</v>
+        <v>10.516</v>
       </c>
       <c r="CT20" s="104">
         <f>IFERROR(VLOOKUP(CS20,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -9814,14 +9834,16 @@
         <f>CONCATENATE(REGISTRATION!C22," ",REGISTRATION!D22," ",REGISTRATION!E22)</f>
         <v>Creus Rondel Ian L</v>
       </c>
-      <c r="D21" s="108"/>
+      <c r="D21" s="108">
+        <v>39</v>
+      </c>
       <c r="E21" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>55.714285714285715</v>
       </c>
       <c r="F21" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16.714285714285715</v>
       </c>
       <c r="G21" s="108"/>
       <c r="H21" s="92" t="e">
@@ -9926,11 +9948,11 @@
       </c>
       <c r="BC21" s="98">
         <f t="shared" si="18"/>
-        <v>13</v>
+        <v>29.714285714285715</v>
       </c>
       <c r="BD21" s="98">
         <f t="shared" si="19"/>
-        <v>13</v>
+        <v>29.71</v>
       </c>
       <c r="BE21" s="108"/>
       <c r="BF21" s="92" t="str">
@@ -10040,7 +10062,7 @@
       </c>
       <c r="CS21" s="104">
         <f t="shared" si="41"/>
-        <v>5.2</v>
+        <v>11.884</v>
       </c>
       <c r="CT21" s="104">
         <f>IFERROR(VLOOKUP(CS21,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -10064,14 +10086,16 @@
         <f>CONCATENATE(REGISTRATION!C23," ",REGISTRATION!D23," ",REGISTRATION!E23)</f>
         <v>Cruz Jovanni P</v>
       </c>
-      <c r="D22" s="108"/>
+      <c r="D22" s="108">
+        <v>38</v>
+      </c>
       <c r="E22" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>54.285714285714285</v>
       </c>
       <c r="F22" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="G22" s="108"/>
       <c r="H22" s="92" t="e">
@@ -10176,11 +10200,11 @@
       </c>
       <c r="BC22" s="98">
         <f t="shared" si="18"/>
-        <v>14</v>
+        <v>30.285714285714285</v>
       </c>
       <c r="BD22" s="98">
         <f t="shared" si="19"/>
-        <v>14</v>
+        <v>30.29</v>
       </c>
       <c r="BE22" s="108"/>
       <c r="BF22" s="92" t="str">
@@ -10290,7 +10314,7 @@
       </c>
       <c r="CS22" s="104">
         <f t="shared" si="41"/>
-        <v>5.6000000000000005</v>
+        <v>12.116</v>
       </c>
       <c r="CT22" s="104">
         <f>IFERROR(VLOOKUP(CS22,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -10314,14 +10338,16 @@
         <f>CONCATENATE(REGISTRATION!C24," ",REGISTRATION!D24," ",REGISTRATION!E24)</f>
         <v>Cruz Tom Russell D</v>
       </c>
-      <c r="D23" s="108"/>
+      <c r="D23" s="108">
+        <v>38</v>
+      </c>
       <c r="E23" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>54.285714285714285</v>
       </c>
       <c r="F23" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="G23" s="108"/>
       <c r="H23" s="92" t="e">
@@ -10426,11 +10452,11 @@
       </c>
       <c r="BC23" s="98">
         <f t="shared" si="18"/>
-        <v>16</v>
+        <v>32.285714285714285</v>
       </c>
       <c r="BD23" s="98">
         <f t="shared" si="19"/>
-        <v>16</v>
+        <v>32.29</v>
       </c>
       <c r="BE23" s="108"/>
       <c r="BF23" s="92" t="str">
@@ -10540,7 +10566,7 @@
       </c>
       <c r="CS23" s="104">
         <f t="shared" ref="CS23:CS70" si="45">IFERROR(((CR23*0.6)+(BD23*0.4)),"")</f>
-        <v>6.4</v>
+        <v>12.916</v>
       </c>
       <c r="CT23" s="104">
         <f>IFERROR(VLOOKUP(CS23,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -10564,14 +10590,16 @@
         <f>CONCATENATE(REGISTRATION!C25," ",REGISTRATION!D25," ",REGISTRATION!E25)</f>
         <v>Cuison Jayson E</v>
       </c>
-      <c r="D24" s="108"/>
+      <c r="D24" s="108">
+        <v>47</v>
+      </c>
       <c r="E24" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>67.142857142857139</v>
       </c>
       <c r="F24" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20.142857142857142</v>
       </c>
       <c r="G24" s="108"/>
       <c r="H24" s="92" t="e">
@@ -10676,11 +10704,11 @@
       </c>
       <c r="BC24" s="98">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>20.142857142857142</v>
       </c>
       <c r="BD24" s="98">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>20.14</v>
       </c>
       <c r="BE24" s="108"/>
       <c r="BF24" s="92" t="str">
@@ -10790,7 +10818,7 @@
       </c>
       <c r="CS24" s="104">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>8.0560000000000009</v>
       </c>
       <c r="CT24" s="104">
         <f>IFERROR(VLOOKUP(CS24,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -10814,14 +10842,16 @@
         <f>CONCATENATE(REGISTRATION!C26," ",REGISTRATION!D26," ",REGISTRATION!E26)</f>
         <v>Espiritu Rasa Lila Dasi R</v>
       </c>
-      <c r="D25" s="108"/>
+      <c r="D25" s="108">
+        <v>50</v>
+      </c>
       <c r="E25" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>71.428571428571431</v>
       </c>
       <c r="F25" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>21.428571428571427</v>
       </c>
       <c r="G25" s="108"/>
       <c r="H25" s="92" t="e">
@@ -10926,11 +10956,11 @@
       </c>
       <c r="BC25" s="98">
         <f t="shared" si="18"/>
-        <v>13</v>
+        <v>34.428571428571431</v>
       </c>
       <c r="BD25" s="98">
         <f t="shared" si="19"/>
-        <v>13</v>
+        <v>34.43</v>
       </c>
       <c r="BE25" s="108"/>
       <c r="BF25" s="92" t="str">
@@ -11040,7 +11070,7 @@
       </c>
       <c r="CS25" s="104">
         <f t="shared" si="45"/>
-        <v>5.2</v>
+        <v>13.772</v>
       </c>
       <c r="CT25" s="104">
         <f>IFERROR(VLOOKUP(CS25,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -11314,14 +11344,16 @@
         <f>CONCATENATE(REGISTRATION!C28," ",REGISTRATION!D28," ",REGISTRATION!E28)</f>
         <v>Jose Carl Russel M</v>
       </c>
-      <c r="D27" s="108"/>
+      <c r="D27" s="108">
+        <v>39</v>
+      </c>
       <c r="E27" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>55.714285714285715</v>
       </c>
       <c r="F27" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16.714285714285715</v>
       </c>
       <c r="G27" s="108"/>
       <c r="H27" s="92" t="e">
@@ -11426,11 +11458,11 @@
       </c>
       <c r="BC27" s="98">
         <f t="shared" si="18"/>
-        <v>15</v>
+        <v>31.714285714285715</v>
       </c>
       <c r="BD27" s="98">
         <f t="shared" si="19"/>
-        <v>15</v>
+        <v>31.71</v>
       </c>
       <c r="BE27" s="108"/>
       <c r="BF27" s="92" t="str">
@@ -11540,7 +11572,7 @@
       </c>
       <c r="CS27" s="104">
         <f t="shared" si="45"/>
-        <v>6</v>
+        <v>12.684000000000001</v>
       </c>
       <c r="CT27" s="104">
         <f>IFERROR(VLOOKUP(CS27,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -11564,14 +11596,16 @@
         <f>CONCATENATE(REGISTRATION!C29," ",REGISTRATION!D29," ",REGISTRATION!E29)</f>
         <v>Jose Ralph Rholwen M</v>
       </c>
-      <c r="D28" s="108"/>
+      <c r="D28" s="108">
+        <v>38</v>
+      </c>
       <c r="E28" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>54.285714285714285</v>
       </c>
       <c r="F28" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="G28" s="108"/>
       <c r="H28" s="92" t="e">
@@ -11676,11 +11710,11 @@
       </c>
       <c r="BC28" s="98">
         <f t="shared" si="18"/>
-        <v>10</v>
+        <v>26.285714285714285</v>
       </c>
       <c r="BD28" s="98">
         <f t="shared" si="19"/>
-        <v>10</v>
+        <v>26.29</v>
       </c>
       <c r="BE28" s="108"/>
       <c r="BF28" s="92" t="str">
@@ -11790,7 +11824,7 @@
       </c>
       <c r="CS28" s="104">
         <f t="shared" si="45"/>
-        <v>4</v>
+        <v>10.516</v>
       </c>
       <c r="CT28" s="104">
         <f>IFERROR(VLOOKUP(CS28,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -12064,14 +12098,16 @@
         <f>CONCATENATE(REGISTRATION!C31," ",REGISTRATION!D31," ",REGISTRATION!E31)</f>
         <v>Masinas Karl Angelo B</v>
       </c>
-      <c r="D30" s="108"/>
+      <c r="D30" s="108">
+        <v>23</v>
+      </c>
       <c r="E30" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>32.857142857142854</v>
       </c>
       <c r="F30" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.8571428571428559</v>
       </c>
       <c r="G30" s="108"/>
       <c r="H30" s="92" t="e">
@@ -12176,11 +12212,11 @@
       </c>
       <c r="BC30" s="98">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>9.8571428571428559</v>
       </c>
       <c r="BD30" s="98">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>9.86</v>
       </c>
       <c r="BE30" s="108"/>
       <c r="BF30" s="92" t="str">
@@ -12290,7 +12326,7 @@
       </c>
       <c r="CS30" s="104">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>3.944</v>
       </c>
       <c r="CT30" s="104">
         <f>IFERROR(VLOOKUP(CS30,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -12314,14 +12350,16 @@
         <f>CONCATENATE(REGISTRATION!C32," ",REGISTRATION!D32," ",REGISTRATION!E32)</f>
         <v>Monzon Almer Ivan C</v>
       </c>
-      <c r="D31" s="108"/>
+      <c r="D31" s="108">
+        <v>38</v>
+      </c>
       <c r="E31" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>54.285714285714285</v>
       </c>
       <c r="F31" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="G31" s="108"/>
       <c r="H31" s="92" t="e">
@@ -12426,11 +12464,11 @@
       </c>
       <c r="BC31" s="98">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="BD31" s="98">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>16.29</v>
       </c>
       <c r="BE31" s="108"/>
       <c r="BF31" s="92" t="str">
@@ -12540,7 +12578,7 @@
       </c>
       <c r="CS31" s="104">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>6.516</v>
       </c>
       <c r="CT31" s="104">
         <f>IFERROR(VLOOKUP(CS31,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -12564,14 +12602,16 @@
         <f>CONCATENATE(REGISTRATION!C33," ",REGISTRATION!D33," ",REGISTRATION!E33)</f>
         <v>Mulitas Jarred R</v>
       </c>
-      <c r="D32" s="108"/>
+      <c r="D32" s="108">
+        <v>41</v>
+      </c>
       <c r="E32" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>58.571428571428577</v>
       </c>
       <c r="F32" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17.571428571428573</v>
       </c>
       <c r="G32" s="108"/>
       <c r="H32" s="92" t="e">
@@ -12676,11 +12716,11 @@
       </c>
       <c r="BC32" s="98">
         <f t="shared" si="18"/>
-        <v>11.000000000000002</v>
+        <v>28.571428571428577</v>
       </c>
       <c r="BD32" s="98">
         <f t="shared" si="19"/>
-        <v>11</v>
+        <v>28.57</v>
       </c>
       <c r="BE32" s="108"/>
       <c r="BF32" s="92" t="str">
@@ -12790,7 +12830,7 @@
       </c>
       <c r="CS32" s="104">
         <f t="shared" si="45"/>
-        <v>4.4000000000000004</v>
+        <v>11.428000000000001</v>
       </c>
       <c r="CT32" s="104">
         <f>IFERROR(VLOOKUP(CS32,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -12814,14 +12854,16 @@
         <f>CONCATENATE(REGISTRATION!C34," ",REGISTRATION!D34," ",REGISTRATION!E34)</f>
         <v>Mullanida Mark Angel B</v>
       </c>
-      <c r="D33" s="108"/>
+      <c r="D33" s="108">
+        <v>60</v>
+      </c>
       <c r="E33" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>85.714285714285708</v>
       </c>
       <c r="F33" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25.714285714285712</v>
       </c>
       <c r="G33" s="108"/>
       <c r="H33" s="92" t="e">
@@ -12926,11 +12968,11 @@
       </c>
       <c r="BC33" s="98">
         <f t="shared" si="18"/>
-        <v>18</v>
+        <v>43.714285714285708</v>
       </c>
       <c r="BD33" s="98">
         <f t="shared" si="19"/>
-        <v>18</v>
+        <v>43.71</v>
       </c>
       <c r="BE33" s="108"/>
       <c r="BF33" s="92" t="str">
@@ -13040,7 +13082,7 @@
       </c>
       <c r="CS33" s="104">
         <f t="shared" si="45"/>
-        <v>7.2</v>
+        <v>17.484000000000002</v>
       </c>
       <c r="CT33" s="104">
         <f>IFERROR(VLOOKUP(CS33,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -13064,14 +13106,16 @@
         <f>CONCATENATE(REGISTRATION!C35," ",REGISTRATION!D35," ",REGISTRATION!E35)</f>
         <v>Noynoyan Bryan Kentt B</v>
       </c>
-      <c r="D34" s="108"/>
+      <c r="D34" s="108">
+        <v>66</v>
+      </c>
       <c r="E34" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>94.285714285714278</v>
       </c>
       <c r="F34" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>28.285714285714281</v>
       </c>
       <c r="G34" s="108"/>
       <c r="H34" s="92" t="e">
@@ -13176,11 +13220,11 @@
       </c>
       <c r="BC34" s="98">
         <f t="shared" si="18"/>
-        <v>17</v>
+        <v>45.285714285714278</v>
       </c>
       <c r="BD34" s="98">
         <f t="shared" si="19"/>
-        <v>17</v>
+        <v>45.29</v>
       </c>
       <c r="BE34" s="108"/>
       <c r="BF34" s="92" t="str">
@@ -13290,7 +13334,7 @@
       </c>
       <c r="CS34" s="104">
         <f t="shared" si="45"/>
-        <v>6.8000000000000007</v>
+        <v>18.116</v>
       </c>
       <c r="CT34" s="104">
         <f>IFERROR(VLOOKUP(CS34,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -13314,14 +13358,16 @@
         <f>CONCATENATE(REGISTRATION!C36," ",REGISTRATION!D36," ",REGISTRATION!E36)</f>
         <v>Ocampo Ryan Daniel V</v>
       </c>
-      <c r="D35" s="108"/>
+      <c r="D35" s="108">
+        <v>28</v>
+      </c>
       <c r="E35" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F35" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G35" s="108"/>
       <c r="H35" s="92" t="e">
@@ -13426,11 +13472,11 @@
       </c>
       <c r="BC35" s="98">
         <f t="shared" si="18"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="BD35" s="98">
         <f t="shared" si="19"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="BE35" s="108"/>
       <c r="BF35" s="92" t="str">
@@ -13540,7 +13586,7 @@
       </c>
       <c r="CS35" s="104">
         <f t="shared" si="45"/>
-        <v>5.6000000000000005</v>
+        <v>10.4</v>
       </c>
       <c r="CT35" s="104">
         <f>IFERROR(VLOOKUP(CS35,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -13564,14 +13610,16 @@
         <f>CONCATENATE(REGISTRATION!C37," ",REGISTRATION!D37," ",REGISTRATION!E37)</f>
         <v>Parianes Kenneth V</v>
       </c>
-      <c r="D36" s="108"/>
+      <c r="D36" s="108">
+        <v>51</v>
+      </c>
       <c r="E36" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>72.857142857142847</v>
       </c>
       <c r="F36" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>21.857142857142854</v>
       </c>
       <c r="G36" s="108"/>
       <c r="H36" s="92" t="e">
@@ -13676,11 +13724,11 @@
       </c>
       <c r="BC36" s="98">
         <f t="shared" si="18"/>
-        <v>14</v>
+        <v>35.857142857142854</v>
       </c>
       <c r="BD36" s="98">
         <f t="shared" si="19"/>
-        <v>14</v>
+        <v>35.86</v>
       </c>
       <c r="BE36" s="108"/>
       <c r="BF36" s="92" t="str">
@@ -13790,7 +13838,7 @@
       </c>
       <c r="CS36" s="104">
         <f t="shared" si="45"/>
-        <v>5.6000000000000005</v>
+        <v>14.344000000000001</v>
       </c>
       <c r="CT36" s="104">
         <f>IFERROR(VLOOKUP(CS36,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -13814,14 +13862,16 @@
         <f>CONCATENATE(REGISTRATION!C38," ",REGISTRATION!D38," ",REGISTRATION!E38)</f>
         <v>Ramos Shaine Marie R</v>
       </c>
-      <c r="D37" s="108"/>
+      <c r="D37" s="108">
+        <v>48</v>
+      </c>
       <c r="E37" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>68.571428571428569</v>
       </c>
       <c r="F37" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20.571428571428569</v>
       </c>
       <c r="G37" s="108"/>
       <c r="H37" s="92" t="e">
@@ -13926,11 +13976,11 @@
       </c>
       <c r="BC37" s="98">
         <f t="shared" si="18"/>
-        <v>11.000000000000002</v>
+        <v>31.571428571428569</v>
       </c>
       <c r="BD37" s="98">
         <f t="shared" si="19"/>
-        <v>11</v>
+        <v>31.57</v>
       </c>
       <c r="BE37" s="108"/>
       <c r="BF37" s="92" t="str">
@@ -14040,7 +14090,7 @@
       </c>
       <c r="CS37" s="104">
         <f t="shared" si="45"/>
-        <v>4.4000000000000004</v>
+        <v>12.628</v>
       </c>
       <c r="CT37" s="104">
         <f>IFERROR(VLOOKUP(CS37,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -14064,14 +14114,16 @@
         <f>CONCATENATE(REGISTRATION!C39," ",REGISTRATION!D39," ",REGISTRATION!E39)</f>
         <v>Ravelo John Dyron B</v>
       </c>
-      <c r="D38" s="108"/>
+      <c r="D38" s="108">
+        <v>38</v>
+      </c>
       <c r="E38" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>54.285714285714285</v>
       </c>
       <c r="F38" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="G38" s="108"/>
       <c r="H38" s="92" t="e">
@@ -14176,11 +14228,11 @@
       </c>
       <c r="BC38" s="98">
         <f t="shared" si="18"/>
-        <v>16</v>
+        <v>32.285714285714285</v>
       </c>
       <c r="BD38" s="98">
         <f t="shared" si="19"/>
-        <v>16</v>
+        <v>32.29</v>
       </c>
       <c r="BE38" s="108"/>
       <c r="BF38" s="92" t="str">
@@ -14290,7 +14342,7 @@
       </c>
       <c r="CS38" s="104">
         <f t="shared" si="45"/>
-        <v>6.4</v>
+        <v>12.916</v>
       </c>
       <c r="CT38" s="104">
         <f>IFERROR(VLOOKUP(CS38,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -14314,14 +14366,16 @@
         <f>CONCATENATE(REGISTRATION!C40," ",REGISTRATION!D40," ",REGISTRATION!E40)</f>
         <v xml:space="preserve">Santos Ariel </v>
       </c>
-      <c r="D39" s="108"/>
+      <c r="D39" s="108">
+        <v>57</v>
+      </c>
       <c r="E39" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>81.428571428571431</v>
       </c>
       <c r="F39" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>24.428571428571427</v>
       </c>
       <c r="G39" s="108"/>
       <c r="H39" s="92" t="e">
@@ -14426,11 +14480,11 @@
       </c>
       <c r="BC39" s="98">
         <f t="shared" si="18"/>
-        <v>15</v>
+        <v>39.428571428571431</v>
       </c>
       <c r="BD39" s="98">
         <f t="shared" si="19"/>
-        <v>15</v>
+        <v>39.43</v>
       </c>
       <c r="BE39" s="108"/>
       <c r="BF39" s="92" t="str">
@@ -14540,7 +14594,7 @@
       </c>
       <c r="CS39" s="104">
         <f t="shared" si="45"/>
-        <v>6</v>
+        <v>15.772</v>
       </c>
       <c r="CT39" s="104">
         <f>IFERROR(VLOOKUP(CS39,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -14564,14 +14618,16 @@
         <f>CONCATENATE(REGISTRATION!C41," ",REGISTRATION!D41," ",REGISTRATION!E41)</f>
         <v>Sibul Mark Anthony B</v>
       </c>
-      <c r="D40" s="108"/>
+      <c r="D40" s="108">
+        <v>35</v>
+      </c>
       <c r="E40" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F40" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G40" s="108"/>
       <c r="H40" s="92" t="e">
@@ -14676,11 +14732,11 @@
       </c>
       <c r="BC40" s="98">
         <f t="shared" si="18"/>
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="BD40" s="98">
         <f t="shared" si="19"/>
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="BE40" s="108"/>
       <c r="BF40" s="92" t="str">
@@ -14790,7 +14846,7 @@
       </c>
       <c r="CS40" s="104">
         <f t="shared" si="45"/>
-        <v>6.4</v>
+        <v>12.4</v>
       </c>
       <c r="CT40" s="104">
         <f>IFERROR(VLOOKUP(CS40,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -14814,14 +14870,16 @@
         <f>CONCATENATE(REGISTRATION!C42," ",REGISTRATION!D42," ",REGISTRATION!E42)</f>
         <v>Videña Cheryl R</v>
       </c>
-      <c r="D41" s="108"/>
+      <c r="D41" s="108">
+        <v>36</v>
+      </c>
       <c r="E41" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>51.428571428571423</v>
       </c>
       <c r="F41" s="95">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15.428571428571427</v>
       </c>
       <c r="G41" s="108"/>
       <c r="H41" s="92" t="e">
@@ -14926,11 +14984,11 @@
       </c>
       <c r="BC41" s="98">
         <f t="shared" si="18"/>
-        <v>7</v>
+        <v>22.428571428571427</v>
       </c>
       <c r="BD41" s="98">
         <f t="shared" si="19"/>
-        <v>7</v>
+        <v>22.43</v>
       </c>
       <c r="BE41" s="108"/>
       <c r="BF41" s="92" t="str">
@@ -15040,7 +15098,7 @@
       </c>
       <c r="CS41" s="104">
         <f t="shared" si="45"/>
-        <v>2.8000000000000003</v>
+        <v>8.9719999999999995</v>
       </c>
       <c r="CT41" s="104">
         <f>IFERROR(VLOOKUP(CS41,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -15064,14 +15122,16 @@
         <f>CONCATENATE(REGISTRATION!C43," ",REGISTRATION!D43," ",REGISTRATION!E43)</f>
         <v>Villamar Raynald M</v>
       </c>
-      <c r="D42" s="108"/>
+      <c r="D42" s="108">
+        <v>39</v>
+      </c>
       <c r="E42" s="92">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>55.714285714285715</v>
       </c>
       <c r="F42" s="95">
         <f t="shared" ref="F42:F70" si="46">IFERROR((E42*$F$7), " ")</f>
-        <v>0</v>
+        <v>16.714285714285715</v>
       </c>
       <c r="G42" s="108"/>
       <c r="H42" s="92" t="e">
@@ -15176,11 +15236,11 @@
       </c>
       <c r="BC42" s="98">
         <f t="shared" si="18"/>
-        <v>8</v>
+        <v>24.714285714285715</v>
       </c>
       <c r="BD42" s="98">
         <f t="shared" si="19"/>
-        <v>8</v>
+        <v>24.71</v>
       </c>
       <c r="BE42" s="108"/>
       <c r="BF42" s="92" t="str">
@@ -15290,7 +15350,7 @@
       </c>
       <c r="CS42" s="104">
         <f t="shared" si="45"/>
-        <v>3.2</v>
+        <v>9.8840000000000003</v>
       </c>
       <c r="CT42" s="104">
         <f>IFERROR(VLOOKUP(CS42,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -22549,7 +22609,7 @@
       </c>
       <c r="C8" s="51">
         <f>'RAW GRADES'!F10</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D8" s="89" t="str">
         <f>'RAW GRADES'!I10</f>
@@ -22569,11 +22629,11 @@
       </c>
       <c r="H8" s="53">
         <f>'RAW GRADES'!BC10</f>
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I8" s="53">
         <f>'RAW GRADES'!BD10</f>
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="J8" s="52" t="str">
         <f>'RAW GRADES'!BK10</f>
@@ -22593,7 +22653,7 @@
       </c>
       <c r="N8" s="55">
         <f>'RAW GRADES'!CS10</f>
-        <v>5.2</v>
+        <v>11.200000000000001</v>
       </c>
       <c r="O8" s="56">
         <f>'RAW GRADES'!CT10</f>
@@ -22614,7 +22674,7 @@
       </c>
       <c r="C9" s="57">
         <f>'RAW GRADES'!F11</f>
-        <v>0</v>
+        <v>14.142857142857141</v>
       </c>
       <c r="D9" s="89" t="str">
         <f>'RAW GRADES'!I11</f>
@@ -22634,11 +22694,11 @@
       </c>
       <c r="H9" s="53">
         <f>'RAW GRADES'!BC11</f>
-        <v>13</v>
+        <v>27.142857142857139</v>
       </c>
       <c r="I9" s="53">
         <f>'RAW GRADES'!BD11</f>
-        <v>13</v>
+        <v>27.14</v>
       </c>
       <c r="J9" s="52" t="str">
         <f>'RAW GRADES'!BK11</f>
@@ -22658,7 +22718,7 @@
       </c>
       <c r="N9" s="58">
         <f>'RAW GRADES'!CS11</f>
-        <v>5.2</v>
+        <v>10.856000000000002</v>
       </c>
       <c r="O9" s="56">
         <f>'RAW GRADES'!CT11</f>
@@ -22679,7 +22739,7 @@
       </c>
       <c r="C10" s="57">
         <f>'RAW GRADES'!F12</f>
-        <v>0</v>
+        <v>24.857142857142858</v>
       </c>
       <c r="D10" s="89" t="str">
         <f>'RAW GRADES'!I12</f>
@@ -22699,11 +22759,11 @@
       </c>
       <c r="H10" s="53">
         <f>'RAW GRADES'!BC12</f>
-        <v>15</v>
+        <v>39.857142857142861</v>
       </c>
       <c r="I10" s="53">
         <f>'RAW GRADES'!BD12</f>
-        <v>15</v>
+        <v>39.86</v>
       </c>
       <c r="J10" s="52" t="str">
         <f>'RAW GRADES'!BK12</f>
@@ -22723,7 +22783,7 @@
       </c>
       <c r="N10" s="58">
         <f>'RAW GRADES'!CS12</f>
-        <v>6</v>
+        <v>15.944000000000001</v>
       </c>
       <c r="O10" s="56">
         <f>'RAW GRADES'!CT12</f>
@@ -22744,7 +22804,7 @@
       </c>
       <c r="C11" s="57">
         <f>'RAW GRADES'!F13</f>
-        <v>0</v>
+        <v>18.857142857142854</v>
       </c>
       <c r="D11" s="89" t="str">
         <f>'RAW GRADES'!I13</f>
@@ -22764,11 +22824,11 @@
       </c>
       <c r="H11" s="53">
         <f>'RAW GRADES'!BC13</f>
-        <v>10</v>
+        <v>28.857142857142854</v>
       </c>
       <c r="I11" s="53">
         <f>'RAW GRADES'!BD13</f>
-        <v>10</v>
+        <v>28.86</v>
       </c>
       <c r="J11" s="52" t="str">
         <f>'RAW GRADES'!BK13</f>
@@ -22788,7 +22848,7 @@
       </c>
       <c r="N11" s="58">
         <f>'RAW GRADES'!CS13</f>
-        <v>4</v>
+        <v>11.544</v>
       </c>
       <c r="O11" s="56">
         <f>'RAW GRADES'!CT13</f>
@@ -22809,7 +22869,7 @@
       </c>
       <c r="C12" s="57">
         <f>'RAW GRADES'!F14</f>
-        <v>0</v>
+        <v>13.714285714285714</v>
       </c>
       <c r="D12" s="89" t="str">
         <f>'RAW GRADES'!I14</f>
@@ -22829,11 +22889,11 @@
       </c>
       <c r="H12" s="53">
         <f>'RAW GRADES'!BC14</f>
-        <v>14</v>
+        <v>27.714285714285715</v>
       </c>
       <c r="I12" s="53">
         <f>'RAW GRADES'!BD14</f>
-        <v>14</v>
+        <v>27.71</v>
       </c>
       <c r="J12" s="52" t="str">
         <f>'RAW GRADES'!BK14</f>
@@ -22853,7 +22913,7 @@
       </c>
       <c r="N12" s="58">
         <f>'RAW GRADES'!CS14</f>
-        <v>5.6000000000000005</v>
+        <v>11.084000000000001</v>
       </c>
       <c r="O12" s="56">
         <f>'RAW GRADES'!CT14</f>
@@ -22874,7 +22934,7 @@
       </c>
       <c r="C13" s="57">
         <f>'RAW GRADES'!F15</f>
-        <v>0</v>
+        <v>18.857142857142854</v>
       </c>
       <c r="D13" s="89" t="str">
         <f>'RAW GRADES'!I15</f>
@@ -22894,11 +22954,11 @@
       </c>
       <c r="H13" s="53">
         <f>'RAW GRADES'!BC15</f>
-        <v>15</v>
+        <v>33.857142857142854</v>
       </c>
       <c r="I13" s="53">
         <f>'RAW GRADES'!BD15</f>
-        <v>15</v>
+        <v>33.86</v>
       </c>
       <c r="J13" s="52" t="str">
         <f>'RAW GRADES'!BK15</f>
@@ -22918,7 +22978,7 @@
       </c>
       <c r="N13" s="58">
         <f>'RAW GRADES'!CS15</f>
-        <v>6</v>
+        <v>13.544</v>
       </c>
       <c r="O13" s="56">
         <f>'RAW GRADES'!CT15</f>
@@ -22939,7 +22999,7 @@
       </c>
       <c r="C14" s="57">
         <f>'RAW GRADES'!F16</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D14" s="89" t="str">
         <f>'RAW GRADES'!I16</f>
@@ -22959,11 +23019,11 @@
       </c>
       <c r="H14" s="53">
         <f>'RAW GRADES'!BC16</f>
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="I14" s="53">
         <f>'RAW GRADES'!BD16</f>
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="J14" s="52" t="str">
         <f>'RAW GRADES'!BK16</f>
@@ -22983,7 +23043,7 @@
       </c>
       <c r="N14" s="58">
         <f>'RAW GRADES'!CS16</f>
-        <v>6.8000000000000007</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="O14" s="56">
         <f>'RAW GRADES'!CT16</f>
@@ -23069,7 +23129,7 @@
       </c>
       <c r="C16" s="57">
         <f>'RAW GRADES'!F18</f>
-        <v>0</v>
+        <v>13.714285714285714</v>
       </c>
       <c r="D16" s="89" t="str">
         <f>'RAW GRADES'!I18</f>
@@ -23089,11 +23149,11 @@
       </c>
       <c r="H16" s="53">
         <f>'RAW GRADES'!BC18</f>
-        <v>0</v>
+        <v>13.714285714285714</v>
       </c>
       <c r="I16" s="53">
         <f>'RAW GRADES'!BD18</f>
-        <v>0</v>
+        <v>13.71</v>
       </c>
       <c r="J16" s="52" t="str">
         <f>'RAW GRADES'!BK18</f>
@@ -23113,7 +23173,7 @@
       </c>
       <c r="N16" s="58">
         <f>'RAW GRADES'!CS18</f>
-        <v>0</v>
+        <v>5.4840000000000009</v>
       </c>
       <c r="O16" s="56">
         <f>'RAW GRADES'!CT18</f>
@@ -23134,7 +23194,7 @@
       </c>
       <c r="C17" s="57">
         <f>'RAW GRADES'!F19</f>
-        <v>0</v>
+        <v>17.142857142857142</v>
       </c>
       <c r="D17" s="89" t="str">
         <f>'RAW GRADES'!I19</f>
@@ -23154,11 +23214,11 @@
       </c>
       <c r="H17" s="53">
         <f>'RAW GRADES'!BC19</f>
-        <v>0</v>
+        <v>17.142857142857142</v>
       </c>
       <c r="I17" s="53">
         <f>'RAW GRADES'!BD19</f>
-        <v>0</v>
+        <v>17.14</v>
       </c>
       <c r="J17" s="52" t="str">
         <f>'RAW GRADES'!BK19</f>
@@ -23178,7 +23238,7 @@
       </c>
       <c r="N17" s="58">
         <f>'RAW GRADES'!CS19</f>
-        <v>0</v>
+        <v>6.8560000000000008</v>
       </c>
       <c r="O17" s="56">
         <f>'RAW GRADES'!CT19</f>
@@ -23199,7 +23259,7 @@
       </c>
       <c r="C18" s="57">
         <f>'RAW GRADES'!F20</f>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="D18" s="89" t="str">
         <f>'RAW GRADES'!I20</f>
@@ -23219,11 +23279,11 @@
       </c>
       <c r="H18" s="53">
         <f>'RAW GRADES'!BC20</f>
-        <v>10</v>
+        <v>26.285714285714285</v>
       </c>
       <c r="I18" s="53">
         <f>'RAW GRADES'!BD20</f>
-        <v>10</v>
+        <v>26.29</v>
       </c>
       <c r="J18" s="52" t="str">
         <f>'RAW GRADES'!BK20</f>
@@ -23243,7 +23303,7 @@
       </c>
       <c r="N18" s="58">
         <f>'RAW GRADES'!CS20</f>
-        <v>4</v>
+        <v>10.516</v>
       </c>
       <c r="O18" s="56">
         <f>'RAW GRADES'!CT20</f>
@@ -23264,7 +23324,7 @@
       </c>
       <c r="C19" s="57">
         <f>'RAW GRADES'!F21</f>
-        <v>0</v>
+        <v>16.714285714285715</v>
       </c>
       <c r="D19" s="89" t="str">
         <f>'RAW GRADES'!I21</f>
@@ -23284,11 +23344,11 @@
       </c>
       <c r="H19" s="53">
         <f>'RAW GRADES'!BC21</f>
-        <v>13</v>
+        <v>29.714285714285715</v>
       </c>
       <c r="I19" s="53">
         <f>'RAW GRADES'!BD21</f>
-        <v>13</v>
+        <v>29.71</v>
       </c>
       <c r="J19" s="52" t="str">
         <f>'RAW GRADES'!BK21</f>
@@ -23308,7 +23368,7 @@
       </c>
       <c r="N19" s="58">
         <f>'RAW GRADES'!CS21</f>
-        <v>5.2</v>
+        <v>11.884</v>
       </c>
       <c r="O19" s="56">
         <f>'RAW GRADES'!CT21</f>
@@ -23329,7 +23389,7 @@
       </c>
       <c r="C20" s="57">
         <f>'RAW GRADES'!F22</f>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="D20" s="89" t="str">
         <f>'RAW GRADES'!I22</f>
@@ -23349,11 +23409,11 @@
       </c>
       <c r="H20" s="53">
         <f>'RAW GRADES'!BC22</f>
-        <v>14</v>
+        <v>30.285714285714285</v>
       </c>
       <c r="I20" s="53">
         <f>'RAW GRADES'!BD22</f>
-        <v>14</v>
+        <v>30.29</v>
       </c>
       <c r="J20" s="52" t="str">
         <f>'RAW GRADES'!BK22</f>
@@ -23373,7 +23433,7 @@
       </c>
       <c r="N20" s="58">
         <f>'RAW GRADES'!CS22</f>
-        <v>5.6000000000000005</v>
+        <v>12.116</v>
       </c>
       <c r="O20" s="56">
         <f>'RAW GRADES'!CT22</f>
@@ -23394,7 +23454,7 @@
       </c>
       <c r="C21" s="57">
         <f>'RAW GRADES'!F23</f>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="D21" s="89" t="str">
         <f>'RAW GRADES'!I23</f>
@@ -23414,11 +23474,11 @@
       </c>
       <c r="H21" s="53">
         <f>'RAW GRADES'!BC23</f>
-        <v>16</v>
+        <v>32.285714285714285</v>
       </c>
       <c r="I21" s="53">
         <f>'RAW GRADES'!BD23</f>
-        <v>16</v>
+        <v>32.29</v>
       </c>
       <c r="J21" s="52" t="str">
         <f>'RAW GRADES'!BK23</f>
@@ -23438,7 +23498,7 @@
       </c>
       <c r="N21" s="58">
         <f>'RAW GRADES'!CS23</f>
-        <v>6.4</v>
+        <v>12.916</v>
       </c>
       <c r="O21" s="56">
         <f>'RAW GRADES'!CT23</f>
@@ -23459,7 +23519,7 @@
       </c>
       <c r="C22" s="57">
         <f>'RAW GRADES'!F24</f>
-        <v>0</v>
+        <v>20.142857142857142</v>
       </c>
       <c r="D22" s="89" t="str">
         <f>'RAW GRADES'!I24</f>
@@ -23479,11 +23539,11 @@
       </c>
       <c r="H22" s="53">
         <f>'RAW GRADES'!BC24</f>
-        <v>0</v>
+        <v>20.142857142857142</v>
       </c>
       <c r="I22" s="53">
         <f>'RAW GRADES'!BD24</f>
-        <v>0</v>
+        <v>20.14</v>
       </c>
       <c r="J22" s="52" t="str">
         <f>'RAW GRADES'!BK24</f>
@@ -23503,7 +23563,7 @@
       </c>
       <c r="N22" s="58">
         <f>'RAW GRADES'!CS24</f>
-        <v>0</v>
+        <v>8.0560000000000009</v>
       </c>
       <c r="O22" s="56">
         <f>'RAW GRADES'!CT24</f>
@@ -23524,7 +23584,7 @@
       </c>
       <c r="C23" s="57">
         <f>'RAW GRADES'!F25</f>
-        <v>0</v>
+        <v>21.428571428571427</v>
       </c>
       <c r="D23" s="89" t="str">
         <f>'RAW GRADES'!I25</f>
@@ -23544,11 +23604,11 @@
       </c>
       <c r="H23" s="53">
         <f>'RAW GRADES'!BC25</f>
-        <v>13</v>
+        <v>34.428571428571431</v>
       </c>
       <c r="I23" s="53">
         <f>'RAW GRADES'!BD25</f>
-        <v>13</v>
+        <v>34.43</v>
       </c>
       <c r="J23" s="52" t="str">
         <f>'RAW GRADES'!BK25</f>
@@ -23568,7 +23628,7 @@
       </c>
       <c r="N23" s="58">
         <f>'RAW GRADES'!CS25</f>
-        <v>5.2</v>
+        <v>13.772</v>
       </c>
       <c r="O23" s="56">
         <f>'RAW GRADES'!CT25</f>
@@ -23654,7 +23714,7 @@
       </c>
       <c r="C25" s="57">
         <f>'RAW GRADES'!F27</f>
-        <v>0</v>
+        <v>16.714285714285715</v>
       </c>
       <c r="D25" s="89" t="str">
         <f>'RAW GRADES'!I27</f>
@@ -23674,11 +23734,11 @@
       </c>
       <c r="H25" s="53">
         <f>'RAW GRADES'!BC27</f>
-        <v>15</v>
+        <v>31.714285714285715</v>
       </c>
       <c r="I25" s="53">
         <f>'RAW GRADES'!BD27</f>
-        <v>15</v>
+        <v>31.71</v>
       </c>
       <c r="J25" s="52" t="str">
         <f>'RAW GRADES'!BK27</f>
@@ -23698,7 +23758,7 @@
       </c>
       <c r="N25" s="58">
         <f>'RAW GRADES'!CS27</f>
-        <v>6</v>
+        <v>12.684000000000001</v>
       </c>
       <c r="O25" s="56">
         <f>'RAW GRADES'!CT27</f>
@@ -23719,7 +23779,7 @@
       </c>
       <c r="C26" s="57">
         <f>'RAW GRADES'!F28</f>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="D26" s="89" t="str">
         <f>'RAW GRADES'!I28</f>
@@ -23739,11 +23799,11 @@
       </c>
       <c r="H26" s="53">
         <f>'RAW GRADES'!BC28</f>
-        <v>10</v>
+        <v>26.285714285714285</v>
       </c>
       <c r="I26" s="53">
         <f>'RAW GRADES'!BD28</f>
-        <v>10</v>
+        <v>26.29</v>
       </c>
       <c r="J26" s="52" t="str">
         <f>'RAW GRADES'!BK28</f>
@@ -23763,7 +23823,7 @@
       </c>
       <c r="N26" s="58">
         <f>'RAW GRADES'!CS28</f>
-        <v>4</v>
+        <v>10.516</v>
       </c>
       <c r="O26" s="56">
         <f>'RAW GRADES'!CT28</f>
@@ -23849,7 +23909,7 @@
       </c>
       <c r="C28" s="57">
         <f>'RAW GRADES'!F30</f>
-        <v>0</v>
+        <v>9.8571428571428559</v>
       </c>
       <c r="D28" s="89" t="str">
         <f>'RAW GRADES'!I30</f>
@@ -23869,11 +23929,11 @@
       </c>
       <c r="H28" s="53">
         <f>'RAW GRADES'!BC30</f>
-        <v>0</v>
+        <v>9.8571428571428559</v>
       </c>
       <c r="I28" s="53">
         <f>'RAW GRADES'!BD30</f>
-        <v>0</v>
+        <v>9.86</v>
       </c>
       <c r="J28" s="52" t="str">
         <f>'RAW GRADES'!BK30</f>
@@ -23893,7 +23953,7 @@
       </c>
       <c r="N28" s="58">
         <f>'RAW GRADES'!CS30</f>
-        <v>0</v>
+        <v>3.944</v>
       </c>
       <c r="O28" s="56">
         <f>'RAW GRADES'!CT30</f>
@@ -23914,7 +23974,7 @@
       </c>
       <c r="C29" s="57">
         <f>'RAW GRADES'!F31</f>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="D29" s="89" t="str">
         <f>'RAW GRADES'!I31</f>
@@ -23934,11 +23994,11 @@
       </c>
       <c r="H29" s="53">
         <f>'RAW GRADES'!BC31</f>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="I29" s="53">
         <f>'RAW GRADES'!BD31</f>
-        <v>0</v>
+        <v>16.29</v>
       </c>
       <c r="J29" s="52" t="str">
         <f>'RAW GRADES'!BK31</f>
@@ -23958,7 +24018,7 @@
       </c>
       <c r="N29" s="58">
         <f>'RAW GRADES'!CS31</f>
-        <v>0</v>
+        <v>6.516</v>
       </c>
       <c r="O29" s="56">
         <f>'RAW GRADES'!CT31</f>
@@ -23979,7 +24039,7 @@
       </c>
       <c r="C30" s="57">
         <f>'RAW GRADES'!F32</f>
-        <v>0</v>
+        <v>17.571428571428573</v>
       </c>
       <c r="D30" s="89" t="str">
         <f>'RAW GRADES'!I32</f>
@@ -23999,11 +24059,11 @@
       </c>
       <c r="H30" s="53">
         <f>'RAW GRADES'!BC32</f>
-        <v>11.000000000000002</v>
+        <v>28.571428571428577</v>
       </c>
       <c r="I30" s="53">
         <f>'RAW GRADES'!BD32</f>
-        <v>11</v>
+        <v>28.57</v>
       </c>
       <c r="J30" s="52" t="str">
         <f>'RAW GRADES'!BK32</f>
@@ -24023,7 +24083,7 @@
       </c>
       <c r="N30" s="58">
         <f>'RAW GRADES'!CS32</f>
-        <v>4.4000000000000004</v>
+        <v>11.428000000000001</v>
       </c>
       <c r="O30" s="56">
         <f>'RAW GRADES'!CT32</f>
@@ -24044,7 +24104,7 @@
       </c>
       <c r="C31" s="57">
         <f>'RAW GRADES'!F33</f>
-        <v>0</v>
+        <v>25.714285714285712</v>
       </c>
       <c r="D31" s="89" t="str">
         <f>'RAW GRADES'!I33</f>
@@ -24064,11 +24124,11 @@
       </c>
       <c r="H31" s="53">
         <f>'RAW GRADES'!BC33</f>
-        <v>18</v>
+        <v>43.714285714285708</v>
       </c>
       <c r="I31" s="53">
         <f>'RAW GRADES'!BD33</f>
-        <v>18</v>
+        <v>43.71</v>
       </c>
       <c r="J31" s="52" t="str">
         <f>'RAW GRADES'!BK33</f>
@@ -24088,7 +24148,7 @@
       </c>
       <c r="N31" s="58">
         <f>'RAW GRADES'!CS33</f>
-        <v>7.2</v>
+        <v>17.484000000000002</v>
       </c>
       <c r="O31" s="56">
         <f>'RAW GRADES'!CT33</f>
@@ -24109,7 +24169,7 @@
       </c>
       <c r="C32" s="57">
         <f>'RAW GRADES'!F34</f>
-        <v>0</v>
+        <v>28.285714285714281</v>
       </c>
       <c r="D32" s="89" t="str">
         <f>'RAW GRADES'!I34</f>
@@ -24129,11 +24189,11 @@
       </c>
       <c r="H32" s="53">
         <f>'RAW GRADES'!BC34</f>
-        <v>17</v>
+        <v>45.285714285714278</v>
       </c>
       <c r="I32" s="53">
         <f>'RAW GRADES'!BD34</f>
-        <v>17</v>
+        <v>45.29</v>
       </c>
       <c r="J32" s="52" t="str">
         <f>'RAW GRADES'!BK34</f>
@@ -24153,7 +24213,7 @@
       </c>
       <c r="N32" s="58">
         <f>'RAW GRADES'!CS34</f>
-        <v>6.8000000000000007</v>
+        <v>18.116</v>
       </c>
       <c r="O32" s="56">
         <f>'RAW GRADES'!CT34</f>
@@ -24174,7 +24234,7 @@
       </c>
       <c r="C33" s="57">
         <f>'RAW GRADES'!F35</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D33" s="89" t="str">
         <f>'RAW GRADES'!I35</f>
@@ -24194,11 +24254,11 @@
       </c>
       <c r="H33" s="53">
         <f>'RAW GRADES'!BC35</f>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="I33" s="53">
         <f>'RAW GRADES'!BD35</f>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="J33" s="52" t="str">
         <f>'RAW GRADES'!BK35</f>
@@ -24218,7 +24278,7 @@
       </c>
       <c r="N33" s="58">
         <f>'RAW GRADES'!CS35</f>
-        <v>5.6000000000000005</v>
+        <v>10.4</v>
       </c>
       <c r="O33" s="56">
         <f>'RAW GRADES'!CT35</f>
@@ -24239,7 +24299,7 @@
       </c>
       <c r="C34" s="57">
         <f>'RAW GRADES'!F36</f>
-        <v>0</v>
+        <v>21.857142857142854</v>
       </c>
       <c r="D34" s="89" t="str">
         <f>'RAW GRADES'!I36</f>
@@ -24259,11 +24319,11 @@
       </c>
       <c r="H34" s="53">
         <f>'RAW GRADES'!BC36</f>
-        <v>14</v>
+        <v>35.857142857142854</v>
       </c>
       <c r="I34" s="53">
         <f>'RAW GRADES'!BD36</f>
-        <v>14</v>
+        <v>35.86</v>
       </c>
       <c r="J34" s="52" t="str">
         <f>'RAW GRADES'!BK36</f>
@@ -24283,7 +24343,7 @@
       </c>
       <c r="N34" s="58">
         <f>'RAW GRADES'!CS36</f>
-        <v>5.6000000000000005</v>
+        <v>14.344000000000001</v>
       </c>
       <c r="O34" s="56">
         <f>'RAW GRADES'!CT36</f>
@@ -24304,7 +24364,7 @@
       </c>
       <c r="C35" s="57">
         <f>'RAW GRADES'!F37</f>
-        <v>0</v>
+        <v>20.571428571428569</v>
       </c>
       <c r="D35" s="89" t="str">
         <f>'RAW GRADES'!I37</f>
@@ -24324,11 +24384,11 @@
       </c>
       <c r="H35" s="53">
         <f>'RAW GRADES'!BC37</f>
-        <v>11.000000000000002</v>
+        <v>31.571428571428569</v>
       </c>
       <c r="I35" s="53">
         <f>'RAW GRADES'!BD37</f>
-        <v>11</v>
+        <v>31.57</v>
       </c>
       <c r="J35" s="52" t="str">
         <f>'RAW GRADES'!BK37</f>
@@ -24348,7 +24408,7 @@
       </c>
       <c r="N35" s="58">
         <f>'RAW GRADES'!CS37</f>
-        <v>4.4000000000000004</v>
+        <v>12.628</v>
       </c>
       <c r="O35" s="56">
         <f>'RAW GRADES'!CT37</f>
@@ -24369,7 +24429,7 @@
       </c>
       <c r="C36" s="57">
         <f>'RAW GRADES'!F38</f>
-        <v>0</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="D36" s="89" t="str">
         <f>'RAW GRADES'!I38</f>
@@ -24389,11 +24449,11 @@
       </c>
       <c r="H36" s="53">
         <f>'RAW GRADES'!BC38</f>
-        <v>16</v>
+        <v>32.285714285714285</v>
       </c>
       <c r="I36" s="53">
         <f>'RAW GRADES'!BD38</f>
-        <v>16</v>
+        <v>32.29</v>
       </c>
       <c r="J36" s="52" t="str">
         <f>'RAW GRADES'!BK38</f>
@@ -24413,7 +24473,7 @@
       </c>
       <c r="N36" s="58">
         <f>'RAW GRADES'!CS38</f>
-        <v>6.4</v>
+        <v>12.916</v>
       </c>
       <c r="O36" s="56">
         <f>'RAW GRADES'!CT38</f>
@@ -24434,7 +24494,7 @@
       </c>
       <c r="C37" s="57">
         <f>'RAW GRADES'!F39</f>
-        <v>0</v>
+        <v>24.428571428571427</v>
       </c>
       <c r="D37" s="89" t="str">
         <f>'RAW GRADES'!I39</f>
@@ -24454,11 +24514,11 @@
       </c>
       <c r="H37" s="53">
         <f>'RAW GRADES'!BC39</f>
-        <v>15</v>
+        <v>39.428571428571431</v>
       </c>
       <c r="I37" s="53">
         <f>'RAW GRADES'!BD39</f>
-        <v>15</v>
+        <v>39.43</v>
       </c>
       <c r="J37" s="52" t="str">
         <f>'RAW GRADES'!BK39</f>
@@ -24478,7 +24538,7 @@
       </c>
       <c r="N37" s="58">
         <f>'RAW GRADES'!CS39</f>
-        <v>6</v>
+        <v>15.772</v>
       </c>
       <c r="O37" s="56">
         <f>'RAW GRADES'!CT39</f>
@@ -24499,7 +24559,7 @@
       </c>
       <c r="C38" s="57">
         <f>'RAW GRADES'!F40</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D38" s="89" t="str">
         <f>'RAW GRADES'!I40</f>
@@ -24519,11 +24579,11 @@
       </c>
       <c r="H38" s="53">
         <f>'RAW GRADES'!BC40</f>
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="I38" s="53">
         <f>'RAW GRADES'!BD40</f>
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="J38" s="52" t="str">
         <f>'RAW GRADES'!BK40</f>
@@ -24543,7 +24603,7 @@
       </c>
       <c r="N38" s="58">
         <f>'RAW GRADES'!CS40</f>
-        <v>6.4</v>
+        <v>12.4</v>
       </c>
       <c r="O38" s="56">
         <f>'RAW GRADES'!CT40</f>
@@ -24564,7 +24624,7 @@
       </c>
       <c r="C39" s="57">
         <f>'RAW GRADES'!F41</f>
-        <v>0</v>
+        <v>15.428571428571427</v>
       </c>
       <c r="D39" s="89" t="str">
         <f>'RAW GRADES'!I41</f>
@@ -24584,11 +24644,11 @@
       </c>
       <c r="H39" s="53">
         <f>'RAW GRADES'!BC41</f>
-        <v>7</v>
+        <v>22.428571428571427</v>
       </c>
       <c r="I39" s="53">
         <f>'RAW GRADES'!BD41</f>
-        <v>7</v>
+        <v>22.43</v>
       </c>
       <c r="J39" s="52" t="str">
         <f>'RAW GRADES'!BK41</f>
@@ -24608,7 +24668,7 @@
       </c>
       <c r="N39" s="58">
         <f>'RAW GRADES'!CS41</f>
-        <v>2.8000000000000003</v>
+        <v>8.9719999999999995</v>
       </c>
       <c r="O39" s="56">
         <f>'RAW GRADES'!CT41</f>
@@ -24629,7 +24689,7 @@
       </c>
       <c r="C40" s="57">
         <f>'RAW GRADES'!F42</f>
-        <v>0</v>
+        <v>16.714285714285715</v>
       </c>
       <c r="D40" s="89" t="str">
         <f>'RAW GRADES'!I42</f>
@@ -24649,11 +24709,11 @@
       </c>
       <c r="H40" s="53">
         <f>'RAW GRADES'!BC42</f>
-        <v>8</v>
+        <v>24.714285714285715</v>
       </c>
       <c r="I40" s="53">
         <f>'RAW GRADES'!BD42</f>
-        <v>8</v>
+        <v>24.71</v>
       </c>
       <c r="J40" s="52" t="str">
         <f>'RAW GRADES'!BK42</f>
@@ -24673,7 +24733,7 @@
       </c>
       <c r="N40" s="58">
         <f>'RAW GRADES'!CS42</f>
-        <v>3.2</v>
+        <v>9.8840000000000003</v>
       </c>
       <c r="O40" s="56">
         <f>'RAW GRADES'!CT42</f>
@@ -28313,7 +28373,7 @@
       <c r="D87" s="60"/>
       <c r="E87" s="246">
         <f ca="1">NOW()</f>
-        <v>43011.57723599537</v>
+        <v>43014.518733449077</v>
       </c>
       <c r="F87" s="246"/>
     </row>

</xml_diff>